<commit_message>
added some c# engine functionality
</commit_message>
<xml_diff>
--- a/ExcelToInsert/ExcelToInsert/TombstoneDb.xlsx
+++ b/ExcelToInsert/ExcelToInsert/TombstoneDb.xlsx
@@ -15,57 +15,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
   <si>
     <t>id (int)</t>
   </si>
   <si>
+    <t>charactername (string)</t>
+  </si>
+  <si>
+    <t>characterdescription (string)</t>
+  </si>
+  <si>
+    <t>locationid (int)</t>
+  </si>
+  <si>
+    <t>Clayton</t>
+  </si>
+  <si>
+    <t>name (string)</t>
+  </si>
+  <si>
+    <t>e (int)</t>
+  </si>
+  <si>
+    <t>w (int)</t>
+  </si>
+  <si>
+    <t>n (int)</t>
+  </si>
+  <si>
+    <t>s (int)</t>
+  </si>
+  <si>
+    <t>description (string)</t>
+  </si>
+  <si>
+    <t>verbosedescription (string)</t>
+  </si>
+  <si>
+    <t>isStart (bool)</t>
+  </si>
+  <si>
+    <t>Office</t>
+  </si>
+  <si>
     <t>playername (string)</t>
   </si>
   <si>
+    <t>The town gaol and your workplace</t>
+  </si>
+  <si>
+    <t>The town gaol and where you spend your long and ultimately unfulfilling existence, before finally passing away without ever leaving any semblance of a mark upon the world. You are a sad, sad person, your life was meaningless. This is a cry for help. Please.</t>
+  </si>
+  <si>
     <t>Jimmy</t>
   </si>
   <si>
-    <t>name (string)</t>
-  </si>
-  <si>
-    <t>e (int)</t>
-  </si>
-  <si>
-    <t>w (int)</t>
-  </si>
-  <si>
-    <t>n (int)</t>
-  </si>
-  <si>
-    <t>s (int)</t>
-  </si>
-  <si>
-    <t>description (string)</t>
-  </si>
-  <si>
-    <t>verbosedescription (string)</t>
-  </si>
-  <si>
-    <t>isStart (bool)</t>
-  </si>
-  <si>
-    <t>Office</t>
-  </si>
-  <si>
-    <t>The town gaol and your workplace</t>
-  </si>
-  <si>
-    <t>The town gaol and where you spend your long and ultimately unfulfilling existence, before finally passing away without ever leaving any semblance of a mark upon the world. You are a sad, sad person, your life was meaningless. This is a cry for help. Please.</t>
-  </si>
-  <si>
     <t>Spooky House</t>
   </si>
   <si>
     <t>An old, run-down house</t>
   </si>
   <si>
-    <t>A spooooooooooky house, run by the ever lovely and elderly Dolores, known for her sweet sweet herbs</t>
+    <t>A spooooooooooky house, run by the ever lovely and elderly Dolores, known for her sweet sweet herbs.</t>
   </si>
   <si>
     <t>Cemetary</t>
@@ -92,19 +104,7 @@
     <t>Where all the rowdy cowboys and cowboy killers walk 'round</t>
   </si>
   <si>
-    <t>Main Street (this is meant to be verbose)</t>
-  </si>
-  <si>
-    <t>charactername (string)</t>
-  </si>
-  <si>
-    <t>characterdescription (string)</t>
-  </si>
-  <si>
-    <t>locationid (int)</t>
-  </si>
-  <si>
-    <t>Clayton</t>
+    <t>Dusty Main Street. A tumbleweed blows slowly by. (this is meant to be verbose)</t>
   </si>
   <si>
     <t>The town drunk and known to be slightly crazy. He is a frequent visitor to the town goal</t>
@@ -131,19 +131,19 @@
     <t>commanddescription (string)</t>
   </si>
   <si>
+    <t>isvisible (bool)</t>
+  </si>
+  <si>
     <t>MOVE</t>
   </si>
   <si>
     <t>move a thing to a place</t>
   </si>
   <si>
-    <t>itemname (string)</t>
-  </si>
-  <si>
-    <t>itemdescription (string)</t>
-  </si>
-  <si>
-    <t>isvisible (bool)</t>
+    <t>TRAVEL(to: location id)</t>
+  </si>
+  <si>
+    <t>travel to a place</t>
   </si>
   <si>
     <t>Dolores's Magic Herbs</t>
@@ -156,6 +156,24 @@
   </si>
   <si>
     <t>A lucky coin, which is well known to belong to Johnny, the sheriff's childhood friend which the player will know somehow</t>
+  </si>
+  <si>
+    <t>William's Gun</t>
+  </si>
+  <si>
+    <t>Nothing special, it's a gun</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Key to the jail cell</t>
+  </si>
+  <si>
+    <t>Door</t>
+  </si>
+  <si>
+    <t>It's a door</t>
   </si>
 </sst>
 </file>
@@ -235,28 +253,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2">
@@ -264,7 +282,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1">
         <v>5.0</v>
@@ -279,10 +297,10 @@
         <v>-1.0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="I2" s="1" t="b">
         <v>1</v>
@@ -293,7 +311,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1">
         <v>-1.0</v>
@@ -308,10 +326,10 @@
         <v>-1.0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="I3" s="1" t="b">
         <v>0</v>
@@ -322,7 +340,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C4" s="1">
         <v>-1.0</v>
@@ -337,10 +355,10 @@
         <v>5.0</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="I4" s="1" t="b">
         <v>0</v>
@@ -351,7 +369,7 @@
         <v>4.0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C5" s="1">
         <v>-1.0</v>
@@ -366,10 +384,10 @@
         <v>-1.0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="I5" s="1" t="b">
         <v>0</v>
@@ -380,7 +398,7 @@
         <v>5.0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C6" s="1">
         <v>4.0</v>
@@ -395,10 +413,10 @@
         <v>2.0</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="I6" s="1" t="b">
         <v>0</v>
@@ -421,7 +439,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2">
@@ -429,7 +447,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -455,13 +473,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2">
@@ -469,7 +487,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>30</v>
@@ -538,7 +556,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>37</v>
@@ -546,10 +564,18 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -576,16 +602,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>41</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2">
@@ -620,6 +646,57 @@
       </c>
       <c r="E3" s="1" t="b">
         <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="E4" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="E5" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="E6" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>